<commit_message>
Unify syntax; add tests
</commit_message>
<xml_diff>
--- a/local-scenarios/cough/processes/ExampleProcess.xlsx
+++ b/local-scenarios/cough/processes/ExampleProcess.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">SELECT * FROM BRANDS</t>
+    <t xml:space="preserve">SELECT * FROM Brands</t>
   </si>
   <si>
     <t xml:space="preserve">What's your previous med brand?</t>
@@ -97,13 +97,34 @@
     <t xml:space="preserve">PreviousMedProduct</t>
   </si>
   <si>
-    <t xml:space="preserve">SELECT * FROM PRODUCT WHERE BrandID == [prev_med_brand]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please choose your {var}{ipa_category} IPA now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ipa_chosen]</t>
+    <t xml:space="preserve">SELECT * FROM Products WHERE brand_id == [prev_med_brand]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please choose your product from the med brand</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GO(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">SeeProduct)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[med]</t>
   </si>
   <si>
     <t xml:space="preserve">SeeProduct</t>
@@ -112,13 +133,31 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
-    <t xml:space="preserve">SELECT * FROM PRODUCT WHERE ID == [some_chosen_product]</t>
+    <t xml:space="preserve">SELECT * FROM Products WHERE id == [med]</t>
   </si>
   <si>
     <t xml:space="preserve">Take a look at this wonderful product</t>
   </si>
   <si>
-    <t xml:space="preserve">GO(Llel), IS_NEXT('lul')</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GO(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FreeText)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FreeText</t>
@@ -128,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gimme answers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINISH()</t>
   </si>
   <si>
     <t xml:space="preserve">[free_text]</t>
@@ -140,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -170,6 +212,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -324,8 +372,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,7 +382,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="60.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.14"/>
   </cols>
@@ -443,7 +491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -456,39 +504,45 @@
       <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>